<commit_message>
Auto-committed on 2023/03/30 週四 17:13:11.37
</commit_message>
<xml_diff>
--- a/Program/Other/L9735_底稿_建商餘額明細.xlsx
+++ b/Program/Other/L9735_底稿_建商餘額明細.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C691011-3EC2-4DE7-AC9B-9E30D73ACAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="yyymmdd" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>戶號</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,13 +75,21 @@
   </si>
   <si>
     <t>撥款日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>評估淨值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>貸放成數</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,21 +418,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="22.5" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="11" width="20.625" style="2" customWidth="1"/>
+    <col min="1" max="11" width="20.59765625" style="2" customWidth="1"/>
     <col min="12" max="16384" width="22.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -464,6 +471,12 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto-committed on 2023/05/02 週二 11:39:02.38
</commit_message>
<xml_diff>
--- a/Program/Other/L9735_底稿_建商餘額明細.xlsx
+++ b/Program/Other/L9735_底稿_建商餘額明細.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA04511-8776-4CC9-BD5F-1A26BA2566F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yyymmdd" sheetId="1" r:id="rId1"/>
@@ -50,10 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上繳日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>擔保品代號1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,12 +81,15 @@
   <si>
     <t>貸放成數</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>繳息迄日</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,12 +418,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:O1"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.5" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -452,31 +452,31 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>